<commit_message>
datasets better and fix user bugs
</commit_message>
<xml_diff>
--- a/Dataset/Datasets/DataSetHeartAtack.xlsx
+++ b/Dataset/Datasets/DataSetHeartAtack.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\ProjectX\Dataset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ICESI\Integrador I\ProjectX\Dataset\Datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E49B2721-6E8A-49E8-8359-BCF6ED15157A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A69CB3B5-21EE-4182-9671-D41A64E24D93}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6F839F34-9887-654D-AC76-FF785A73B725}"/>
   </bookViews>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D88DF22F-A81F-F346-AED9-7C608A3D80B1}">
   <dimension ref="A1:K304"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A304"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="60" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:XFD201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>